<commit_message>
2022-10-04 Work with network: traceroute
</commit_message>
<xml_diff>
--- a/GNU_Linux/Linux_Architecture/FileSystem_root.xlsx
+++ b/GNU_Linux/Linux_Architecture/FileSystem_root.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Краткое описание хранящихся файлов</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>/srv</t>
-  </si>
-  <si>
-    <t>исполняемые файлы</t>
   </si>
   <si>
     <t>файлы устройств</t>
@@ -267,12 +264,6 @@
   </si>
   <si>
     <t>(=optional applications) дополнительные программы</t>
-  </si>
-  <si>
-    <t>в эту папку устанавливаются проприетарные программы, игры или драйвера.
-Это программы созданные в виде отдельных исполняемых файлов самими производителями. 
-Такие программы устанавливаются в под-каталоги /opt/ 
-все исполняемые файлы, библиотеки и файлы конфигурации находятся в одной папке.</t>
   </si>
   <si>
     <t>в этот каталог можно монтировать внешние или дополнительные файловые системы</t>
@@ -994,6 +985,18 @@
       <t xml:space="preserve">
 Кроме файлов в этом каталоге есть большая структура папок linux, из которых можно узнать достаточно много информации о системе</t>
     </r>
+  </si>
+  <si>
+    <t>исполняемые файлы для настройки ОС</t>
+  </si>
+  <si>
+    <t>исполняемые файлы, используемые всеми пользователями</t>
+  </si>
+  <si>
+    <t>в эту папку устанавливаются проприетарные программы, игры или драйвера.
+Это программы созданные в виде отдельных исполняемых файлов самими производителями. 
+Такие программы устанавливаются в подкаталоги /opt/ 
+все исполняемые файлы, библиотеки и файлы конфигурации находятся в одной папке.</t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="145" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1519,13 +1522,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="13"/>
     </row>
@@ -1534,13 +1537,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1548,11 +1551,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
@@ -1560,11 +1563,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1572,11 +1575,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -1584,11 +1587,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1596,11 +1599,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1608,11 +1611,11 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="242.25" x14ac:dyDescent="0.25">
@@ -1620,13 +1623,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
@@ -1634,11 +1637,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -1646,11 +1649,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="63" x14ac:dyDescent="0.25">
@@ -1658,11 +1661,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="175.5" x14ac:dyDescent="0.25">
@@ -1670,11 +1673,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -1682,13 +1685,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,13 +1699,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1710,11 +1713,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
@@ -1722,11 +1725,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
@@ -1734,11 +1737,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -1746,11 +1749,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>